<commit_message>
refix: barcodes and excel files for editing action, editing price. Feat: fbo get warehouse balances
</commit_message>
<xml_diff>
--- a/src/assets/categories.xlsx
+++ b/src/assets/categories.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ЭтаКнига"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\Программы\Самописные\All_Programs\sales\dist\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prog\Desktop\Programs\best-hub-server\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{057BFF6C-7943-46DF-B2EA-3D2DF7DB667C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5555D8B7-E2ED-4532-A32B-A2EC36A1250A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="588">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="595" uniqueCount="589">
   <si>
     <t>22-бордовый</t>
   </si>
@@ -1799,6 +1799,9 @@
   </si>
   <si>
     <t>лето сабо</t>
+  </si>
+  <si>
+    <t>Стандартная комиссия озон:</t>
   </si>
 </sst>
 </file>
@@ -1940,7 +1943,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -1982,6 +1985,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Нейтральный" xfId="1" builtinId="28"/>
@@ -2327,8 +2331,8 @@
   <sheetPr codeName="Лист1"/>
   <dimension ref="A1:R562"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="S20" sqref="S20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2346,7 +2350,7 @@
     <col min="12" max="12" width="16.85546875" customWidth="1"/>
     <col min="14" max="14" width="9.28515625" customWidth="1"/>
     <col min="15" max="15" width="12.42578125" style="12" customWidth="1"/>
-    <col min="16" max="16" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="27.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2506,7 +2510,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>144</v>
       </c>
@@ -2551,6 +2555,15 @@
       </c>
       <c r="O4" s="12">
         <v>500</v>
+      </c>
+      <c r="P4" s="21" t="s">
+        <v>588</v>
+      </c>
+      <c r="Q4" s="10">
+        <v>25</v>
+      </c>
+      <c r="R4" s="11" t="s">
+        <v>362</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">

</xml_diff>